<commit_message>
Backup folder - 2023-10-24 19:08:15
</commit_message>
<xml_diff>
--- a/UI:UX Design/Lab_2/Персонажі.xlsx
+++ b/UI:UX Design/Lab_2/Персонажі.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yarik/Desktop/✈️ ХАІ 💻/UI:UX Design/Lab_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77531122-D8BD-A541-8C9D-D2447C5A26D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48425406-5979-964A-8EB1-20734B2F5C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{29B7939F-A647-B04E-9E94-5BB5B9DA63AE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{29B7939F-A647-B04E-9E94-5BB5B9DA63AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="2" r:id="rId1"/>
     <sheet name="Лист2" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$D$8</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>Світлина</t>
   </si>
@@ -80,9 +83,6 @@
     <t>Ольга, 50 років, вміє швидко зводити дебет з кредитом, любить готувати нові страви для своєї сімʼї</t>
   </si>
   <si>
-    <t>Мені не подобається Photoshop, оскільки в ньому забагато функцій, і мало що інтуіїтивно зрозуміло. Хочеться більше витрачати часу на реалізацію ідеї, а не вивчення кнопочок</t>
-  </si>
-  <si>
     <t>Простійший та зрозуміліший інтерфейс; модульне завантаження редактору</t>
   </si>
   <si>
@@ -107,9 +107,6 @@
     <t>Показати переваги платної підписки на сервіс, показати зручний інтерфейс та відповідність всім побажанням Марії</t>
   </si>
   <si>
-    <t>швидко знаходить потрібні йому інструменти та розуміє як з ними працювати по бібліотеці відео з прикладами використання. Пробує нові можливості ШІ</t>
-  </si>
-  <si>
     <t>За допомогою пошуку швидко знаходить потрібну персону чи інформацію та може її відфільтрувати по категоріям</t>
   </si>
   <si>
@@ -131,7 +128,22 @@
     <t>Бухгалтер в крупному гіпермаркеті</t>
   </si>
   <si>
-    <t xml:space="preserve">Потрібен хороший аналог 1С. Оскільки 1С в деяких моментах забирав багато часу, хочеться щоб це виправили у новій програмі </t>
+    <t>Мені не подобається стояти в черзі за квитками, хочеться переглянути опис та відгуки людей на театральну постанову, перед тим як відвідувати</t>
+  </si>
+  <si>
+    <t>При оплаті квитків виникають труднощі, оскільки немає зручного способу оплати чи інструкції з оплати</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> На веб-сайті сервісу недостатньо інформації про графік вистав, що ускладнює вибір</t>
+  </si>
+  <si>
+    <t>Швидке оформлення квитків онлайн, попередню інформацію про подію</t>
+  </si>
+  <si>
+    <t>Напівавтоматичний платіж через мобільний банкінг або сервіси оплати GPay та Apple Pay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Детальна інформація про графік театральних вистав, включаючи дати, часи і описи. </t>
   </si>
 </sst>
 </file>
@@ -168,7 +180,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -176,17 +188,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -210,15 +238,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:colOff>355600</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:colOff>1587500</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1524000</xdr:rowOff>
+      <xdr:rowOff>1640558</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -247,8 +275,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1206500" y="25400"/>
-          <a:ext cx="1143000" cy="1498600"/>
+          <a:off x="1181100" y="25400"/>
+          <a:ext cx="1231900" cy="1615158"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -260,15 +288,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>130427</xdr:colOff>
+      <xdr:colOff>112069</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1587500</xdr:colOff>
+      <xdr:colOff>1625601</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1552734</xdr:rowOff>
+      <xdr:rowOff>1638300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -297,8 +325,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2899027" y="0"/>
-          <a:ext cx="1457073" cy="1552734"/>
+          <a:off x="2880669" y="25400"/>
+          <a:ext cx="1513532" cy="1612900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -310,15 +338,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>176310</xdr:colOff>
+      <xdr:colOff>189010</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1490</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1548620</xdr:colOff>
+      <xdr:colOff>1561320</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1557063</xdr:rowOff>
+      <xdr:rowOff>1638300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -346,8 +374,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4697510" y="1490"/>
-          <a:ext cx="1372310" cy="1555573"/>
+          <a:off x="4710210" y="1490"/>
+          <a:ext cx="1372310" cy="1636810"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -364,15 +392,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:colOff>84665</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>592668</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>799461</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>2082800</xdr:rowOff>
+      <xdr:rowOff>1661584</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -401,8 +429,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12700" y="541867"/>
-          <a:ext cx="1384300" cy="2070100"/>
+          <a:off x="84665" y="1121835"/>
+          <a:ext cx="714796" cy="1068916"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -414,15 +442,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>12699</xdr:colOff>
+      <xdr:colOff>76199</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>453408</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1385671</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>1676908</xdr:rowOff>
+      <xdr:rowOff>1348823</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -451,8 +479,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12699" y="2628900"/>
-          <a:ext cx="1372972" cy="1664208"/>
+          <a:off x="76199" y="3226241"/>
+          <a:ext cx="738718" cy="895415"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -464,15 +492,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>11210</xdr:colOff>
+      <xdr:colOff>85292</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>14190</xdr:rowOff>
+      <xdr:rowOff>232835</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1383520</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1754</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1887263</xdr:rowOff>
+      <xdr:rowOff>1231098</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -488,7 +516,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -500,8 +528,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11210" y="4320838"/>
-          <a:ext cx="1372310" cy="1873073"/>
+          <a:off x="85292" y="4857752"/>
+          <a:ext cx="731379" cy="998263"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -813,116 +841,120 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="124" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="130" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" ht="34" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="63" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="97" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="63" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="108" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="68" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="113" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="78" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="113" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="109" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="100" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="1" t="s">
+    <row r="8" spans="1:4" ht="94" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="126" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
+      <c r="D8" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -937,115 +969,117 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43E9662E-355E-124F-ABAB-07B0172578A3}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="1" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
     <col min="6" max="6" width="18.83203125" customWidth="1"/>
-    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
     <col min="8" max="8" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="42" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="164" customHeight="1">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:8" ht="177" customHeight="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="146" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="124" customHeight="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="133" customHeight="1">
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="150" customHeight="1">
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backup folder - 2023-10-24 19:59:14
</commit_message>
<xml_diff>
--- a/UI:UX Design/Lab_2/Персонажі.xlsx
+++ b/UI:UX Design/Lab_2/Персонажі.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yarik/Desktop/✈️ ХАІ 💻/UI:UX Design/Lab_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48425406-5979-964A-8EB1-20734B2F5C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0012D1-672C-7B4F-9A2B-3C236C2048F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{29B7939F-A647-B04E-9E94-5BB5B9DA63AE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>Світлина</t>
   </si>
@@ -144,6 +144,33 @@
   </si>
   <si>
     <t xml:space="preserve">Детальна інформація про графік театральних вистав, включаючи дати, часи і описи. </t>
+  </si>
+  <si>
+    <t>Показати швидікість та зручність оформлення покупки квитків та зручність пізнання інформації</t>
+  </si>
+  <si>
+    <t>Показати легку оплату за допомогою P24, MonoDirect, LiqPay, pay.Fondy.ua, GPay та Apple Pay</t>
+  </si>
+  <si>
+    <t>Обирає виставу яка сподобалась, обирає дату та оплачує квиток</t>
+  </si>
+  <si>
+    <t>Обирає виставу яка сподобалась, переглядає опис події, потім обирає дату та оплачує квиток</t>
+  </si>
+  <si>
+    <t>Дуже уважно читає інструкцію з оплати. Перший раз вводить номер карти вручну, що не дуже безпечно, та не дуже швидко</t>
+  </si>
+  <si>
+    <t>Користується підключеним екваерінгом до сервісу,ввести тільки номер телефону та підтвердити запит на оплату в мобільному банкінгу</t>
+  </si>
+  <si>
+    <t>Показати календар з детальним та зручним графіком вистав, та зручним переходом до сторінки з виставою</t>
+  </si>
+  <si>
+    <t>Обрала виставу та змогла переглянути в календарі, коли ще будуть постановки цієї вистави</t>
+  </si>
+  <si>
+    <t>Корегує свої плани на тиждень, коли зʼявляється цікава постанова. Може обрати зручний для себе день</t>
   </si>
 </sst>
 </file>
@@ -840,15 +867,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6125B3A9-A458-D34A-BA8B-2C7A0E7777BC}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="4" width="23" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="130" customHeight="1">
@@ -887,7 +915,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="97" customHeight="1">
+    <row r="4" spans="1:4" ht="123" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -920,27 +948,27 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="109" customHeight="1">
+    <row r="7" spans="1:4" ht="98" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="94" customHeight="1">
@@ -948,13 +976,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>